<commit_message>
CC user and TL user execution commit
</commit_message>
<xml_diff>
--- a/cucumberframework/InputExcelData/ConvertLead.xlsx
+++ b/cucumberframework/InputExcelData/ConvertLead.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CucumberFramework-master\CucumberFramework-master\InputExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\TouchPointFramework\TouchPointFramework\cucumberframework\InputExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2454667B-FE0E-4CFD-90F7-F6CA030BFA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F549047E-7C2D-4A95-8B33-634A60BFE3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Bbtest Us</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Bbtest UsS</t>
+  </si>
+  <si>
+    <t>Apple Test User</t>
+  </si>
+  <si>
+    <t>Tim Tailor</t>
+  </si>
+  <si>
+    <t>BbSalesAgent</t>
+  </si>
+  <si>
+    <t>TlSalesAgent</t>
+  </si>
+  <si>
+    <t>CcSalesAgent</t>
+  </si>
+  <si>
+    <t>James Crafty</t>
   </si>
 </sst>
 </file>
@@ -372,34 +384,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Non billable code commit
</commit_message>
<xml_diff>
--- a/cucumberframework/InputExcelData/ConvertLead.xlsx
+++ b/cucumberframework/InputExcelData/ConvertLead.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\TouchPointFramework\TouchPointFramework\cucumberframework\InputExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F549047E-7C2D-4A95-8B33-634A60BFE3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8CCDE6-58DE-4E71-8AA5-0ADB844BCAEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Bbtest UsS</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>James Crafty</t>
+  </si>
+  <si>
+    <t>Amelia-Test Soriano</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>

</xml_diff>